<commit_message>
MLP working, plots charted and dataset filters improved
</commit_message>
<xml_diff>
--- a/resultados/resultados_forest.xlsx
+++ b/resultados/resultados_forest.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -646,6 +646,27 @@
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
     </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>10</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>number_of_seasons</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0.763870780420232</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.2072117123926988</v>
+      </c>
+      <c r="E10" t="n">
+        <v>100</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>